<commit_message>
Site updated: 2025年9月17日 23:11:45
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE263D9C-F287-40BC-B497-45934E67282D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238C930A-C47F-487A-9D90-0AE7FC6B93DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>The Red Union had been attacking the headquarters of the April Twenty-eighth Brigade for two days. Their red flags fluttered restlessly around the brigade building like flames yearning for firewood.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -195,13 +195,133 @@
   <si>
     <t>每次他们都能在弹雨中全身而退，为自己挣到崇高的荣誉。这次出来的女孩儿显然也相信自己还有那样的幸运。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_010</t>
+  </si>
+  <si>
+    <t>She waved the battle banner as though brandishing her burning youth, trusting that the enemy would be burnt to ashes in the revolutionary flames, imagining that an ideal world would be born tomorrow from the ardor and zeal coursing through her blood.…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>她挥舞着战旗，仿佛挥舞着她燃烧的青春，相信敌人将在革命的火焰中被烧成灰烬，想象着一个理想的世界将从她血液中流淌的热情和激情中诞生</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>…</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>她挥舞着战旗，挥动着自己燃烧的青春，敌人将在这火焰中化为灰烬，理想世界明天就会在她那沸腾的热血中诞生</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>……</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>She was intoxicated by her brilliant, crimson dream until a bullet pierced her chest. Her fifteen-year-old body was so soft that the bullet hardly slowed down as it passed through it and whistled in the air behind her.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>她陶醉在这鲜红灿烂的梦幻中，直到被一颗步枪子弹洞穿了胸膛，十五岁少女的胸膛是那么柔嫩，那颗子弹穿过后基本上没有减速，在她身后的空中发出一声啾鸣。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The young Red Guard tumbled down along with her flag, her light form descending even more slowly than the piece of red fabric, like a little bird unwilling to leave the sky.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">The Red Union warriors shouted in joy. A few rushed to the foot of the building, tore away the battle banner of the April Twenty-eighth Brigade, and seized the slender, lifeless body. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>They raised their trophy overhead and flaunted it for a while before tossing it toward the top of the metal gate of the compound.</t>
+  </si>
+  <si>
+    <t>Most of the gate’s metal bars, capped with sharp tips, had been pulled down at the beginning of the factional civil wars to be used as spears, but two still remained. As their sharp tips caught the girl, life seemed to return momentarily to her body.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Red Guards backed up some distance and began to use the impaled body for target practice. For her, the dense storm of bullets was now no different from a gentle rain, as she could no longer feel anything.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>From time to time, her vinelike arms jerked across her body softly, as though she were flicking off drops of rain.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>And then half of her young head was blown away, and only a single, beautiful eye remained to stare at the blue sky of 1967. There was no pain in that gaze, only solidified devotion and yearning.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>And yet, compared to some others, she was fortunate. At least she died in the throes of passionately sacrificing herself for an ideal.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_011</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_012</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_013</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_014</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_015</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_016</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_017</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_018</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_019</t>
+  </si>
+  <si>
+    <t>年轻的红卫兵同她的旗帜一起从楼顶落下，她那轻盈的身体落得甚至比旗帜还慢，仿佛小鸟眷恋着天空。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +355,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -256,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -268,6 +395,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -550,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -702,6 +832,116 @@
         <v>20</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2.1412037037037038E-3</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.3379629629629631E-3</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2.3379629629629631E-3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2.5347222222222221E-3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2.5347222222222221E-3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2.685185185185185E-3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2025年9月19日 00:45:24
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238C930A-C47F-487A-9D90-0AE7FC6B93DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED54918-FAFF-40DD-8EF3-770AAA9E4E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>The Red Union had been attacking the headquarters of the April Twenty-eighth Brigade for two days. Their red flags fluttered restlessly around the brigade building like flames yearning for firewood.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -315,6 +315,10 @@
   </si>
   <si>
     <t>年轻的红卫兵同她的旗帜一起从楼顶落下，她那轻盈的身体落得甚至比旗帜还慢，仿佛小鸟眷恋着天空。</t>
+  </si>
+  <si>
+    <t>她陶醉在她灿烂的、深红色的梦里，直到一颗子弹穿透了她的胸膛。她十五岁的身体如此柔软，子弹穿过身体时几乎没有减速，在她身后的空气中呼啸而过。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -683,7 +687,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -868,6 +872,9 @@
       <c r="E11" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="F11" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">

</xml_diff>

<commit_message>
Site updated: 2025年9月21日 00:39:28
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED54918-FAFF-40DD-8EF3-770AAA9E4E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B627978F-9C95-4BD2-AFAD-FDA7D6A6081C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>The Red Union had been attacking the headquarters of the April Twenty-eighth Brigade for two days. Their red flags fluttered restlessly around the brigade building like flames yearning for firewood.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -260,25 +260,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">The Red Union warriors shouted in joy. A few rushed to the foot of the building, tore away the battle banner of the April Twenty-eighth Brigade, and seized the slender, lifeless body. </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>They raised their trophy overhead and flaunted it for a while before tossing it toward the top of the metal gate of the compound.</t>
-  </si>
-  <si>
     <t>Most of the gate’s metal bars, capped with sharp tips, had been pulled down at the beginning of the factional civil wars to be used as spears, but two still remained. As their sharp tips caught the girl, life seemed to return momentarily to her body.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>The Red Guards backed up some distance and began to use the impaled body for target practice. For her, the dense storm of bullets was now no different from a gentle rain, as she could no longer feel anything.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>From time to time, her vinelike arms jerked across her body softly, as though she were flicking off drops of rain.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>And then half of her young head was blown away, and only a single, beautiful eye remained to stare at the blue sky of 1967. There was no pain in that gaze, only solidified devotion and yearning.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -308,16 +293,108 @@
     <t>01_The_Madness_Years_017</t>
   </si>
   <si>
-    <t>01_The_Madness_Years_018</t>
-  </si>
-  <si>
-    <t>01_The_Madness_Years_019</t>
+    <t>她陶醉在她灿烂的、深红色的梦里，直到一颗子弹穿透了她的胸膛。她十五岁的身体如此柔软，子弹穿过身体时几乎没有减速，在她身后的空气中呼啸而过。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年轻的红卫兵和她的旗帜一起坠落，她的身影比那块红色的布料下降得还要慢，就像一只不愿离开天空的小鸟。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>年轻的红卫兵同她的旗帜一起从楼顶落下，她那轻盈的身体落得甚至比旗帜还慢，仿佛小鸟眷恋着天空。</t>
-  </si>
-  <si>
-    <t>她陶醉在她灿烂的、深红色的梦里，直到一颗子弹穿透了她的胸膛。她十五岁的身体如此柔软，子弹穿过身体时几乎没有减速，在她身后的空气中呼啸而过。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Red Union warriors shouted in joy. A few rushed to the foot of the building, tore away the battle banner of the April Twenty-eighth Brigade, and seized the slender, lifeless body. They raised their trophy overhead and flaunted it for a while before tossing it toward the top of the metal gate of the compound.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红色联盟的战士们欢呼着。有几个冲到楼脚下，扯掉了四二八旅的战斗旗帜，抓住了那具瘦长的、毫无生气的尸体。他们将奖杯举过头顶，炫耀了一会儿，然后将它抛向大院金属大门的顶部。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The Red Guards backed up some distance and began to use the impaled body for target practice. For her, the dense storm of bullets was now no different from a gentle rain, as she could no longer feel anything. From time to time, her vinelike arms jerked across her body softly, as though she were flicking off drops of rain.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大多数大门的金属杆，顶端都是尖尖的，在派系内战开始时被拉下来当长矛用，但是还有两根保留了下来。当它们锋利的尖端抓住女孩时，生命似乎瞬间回到了她的身体。</t>
+  </si>
+  <si>
+    <t>红卫兵后退了一段距离，开始用被刺穿的身体进行打靶练习。对她来说，密集的枪林弹雨现在和轻柔的雨没什么不同，因为她再也感觉不到任何东西了。她像醋一样的手臂不时轻轻地在身上晃动，仿佛在拂去雨滴。</t>
+  </si>
+  <si>
+    <r>
+      <t>接着，她年轻的半个脑袋被炸掉了，只剩下一只美丽的眼睛凝视着</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1967</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>年的蓝天。那目光里没有痛苦，只有凝固的虔诚和向往。</t>
+    </r>
+  </si>
+  <si>
+    <t>然而，与其他人相比，她是幸运的。至少她死于为理想而热情牺牲自己的痛苦中。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红色联合的战士们欢呼起来，几个人冲到楼下，掀开四</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二八的旗帜，抬起下面纤小的遗体，做为一个战利品炫耀地举了一段，然后将她高高地扔向大院的铁门。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁门上带尖的金属栅条大部分在武斗初期就被抽走当梭镖了，剩下的两条正好挂住了她，那一瞬间，生命似乎又回到了那个柔软的躯体。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红色联合的红卫兵们退后一段距离，将那个挂在高处的躯体当靶子练习射击，密集的子弹对她来说已柔和如雨，不再带来任何感觉，她那春藤般的手臂不时轻挥一下，仿佛拂去落在身上的雨滴。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直到那颗年轻的头颅被打掉了一半，仅剩的一只美丽的眼睛仍然凝视着一九六七年的蓝天，目光中没有痛苦，只有凝固的激情和渴望。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其实，比起另外一些人来，她还是幸运的，至少是在为理想献身的壮丽激情中死去。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -684,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -864,7 +941,7 @@
         <v>2.5347222222222221E-3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>26</v>
@@ -873,7 +950,7 @@
         <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -884,69 +961,116 @@
         <v>2.685185185185185E-3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2.6967592592592594E-3</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.9050925925925928E-3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2.9050925925925928E-3</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.1018518518518517E-3</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3.1134259259259257E-3</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.3680555555555556E-3</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>3.3680555555555556E-3</v>
+      </c>
+      <c r="B16" s="1">
+        <v>3.5648148148148149E-3</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3.5763888888888889E-3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3.7152777777777778E-3</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>35</v>
+      <c r="E17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2025年9月22日 01:40:26
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B627978F-9C95-4BD2-AFAD-FDA7D6A6081C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46443903-9CE8-4059-94E5-532D6BA0D4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,7 +764,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Site updated: 2025年9月23日 22:53:26
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46443903-9CE8-4059-94E5-532D6BA0D4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE7BB8-378D-4A2C-AA14-2B0B025CC375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>The Red Union had been attacking the headquarters of the April Twenty-eighth Brigade for two days. Their red flags fluttered restlessly around the brigade building like flames yearning for firewood.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -395,6 +395,226 @@
   </si>
   <si>
     <t>其实，比起另外一些人来，她还是幸运的，至少是在为理想献身的壮丽激情中死去。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Battles like this one raged across Beijing like a multitude of CPUs working in parallel, their combined output, the Cultural Revolution. A flood of madness drowned the city and seeped into every nook and cranny.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>At the edge of the city, on the exercise grounds of Tsinghua University, a mass “struggle session” attended by thousands had been going on for nearly two hours.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>This was a public rally intended to humiliate and break down the enemies of the revolution through verbal and physical abuse until they confessed to their crimes before the crowd.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">As the revolutionaries had splintered into numerous factions, opposing forces everywhere engaged in complex maneuvers and contests. Within the university, intense conflicts erupted between the Red Guards, the Cultural Revolution Working Group, the Workers’ Propaganda Team, and the Military Propaganda Team. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>And each faction divided into new rebel groups from time to time, each based on different backgrounds and agendas, leading to even more ruthless fighting.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>But for this mass struggle session, the victims were the reactionary bourgeois academic authorities. These were the enemies of every faction, and they had no choice but to endure cruel attacks from every side.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Compared to other “Monsters and Demons,” reactionary academic authorities were special: During the earliest struggle sessions, they had been both arrogant and stubborn. That was also the stage in which they had died in the largest numbers. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Over a period of forty days, in Beijing alone, more than seventeen hundred victims of struggle sessions were beaten to death. Many others picked an easier path to avoid the madness: Lao She, Wu Han, Jian Bozan, Fu Lei, Zhao Jiuzhang, Yi Qun, Wen Jie, Hai Mo, and other once-respected intellectuals had all chosen to end their lives.3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Those who survived that initial period gradually became numb as the ruthless struggle sessions continued. The protective mental shell helped them avoid total breakdown.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>They often seemed to be half asleep during the sessions and would only startle awake when someone screamed in their faces to make them mechanically recite their confessions, already repeated countless times.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Then, some of them entered a third stage. The constant, unceasing struggle sessions injected vivid political images into their consciousness like mercury, until their minds, erected upon knowledge and rationality, collapsed under the assault. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>They began to really believe that they were guilty, to see how they had harmed the great cause of the revolution. They cried, and their repentance was far deeper and more sincere than that of those Monsters and Demons who were not intellectuals.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">For the Red Guards, heaping abuse upon victims in those two latter mental stages was utterly boring. Only those Monsters and Demons who were still in the initial stage could give their overstimulated brains the thrill they craved, like the red cape of the matador. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>But such desirable victims had grown scarce. In Tsinghua there was probably only one left. Because he was so rare, he was reserved for the very end of the struggle session.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_018</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_019</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_020</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_021</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_022</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_023</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_024</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_025</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_026</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_027</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_028</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_029</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_030</t>
+  </si>
+  <si>
+    <t>01_The_Madness_Years_031</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>这样的热点遍布整座城市，像无数并行运算的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CPU</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，将</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>文化大革命</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>联为一个整体。疯狂如同无形的洪水，将城市淹没其中，并渗透到每一个细微的角落和缝隙。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在城市边缘的那所著名大学的操场上，一场几千人参加的批斗会已经进行了近两个小时。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在这个派别林立的年代，任何一处都有错综复杂的对立派别在格斗。在校园中，红卫兵、文革工作组、工宣队和军宣队，相互之间都在爆发尖锐的冲突，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>而每种派别的内部又时时分化出新的对立派系，捍卫着各自不同的背景和纲领，爆发更为残酷的较量。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>但这次被批斗的反动学术权威，却是任何一方均无异议的斗争目标，他们也只能同时承受来自各方的残酷打击。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与其他牛鬼蛇神相比，反动学术权威有他们的特点：当打击最初到来时，他们的表现往往是高傲而顽固的，这也是他们伤亡率最高的阶段；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在首都，四十天的时间里就有一千七百多名批斗对象被活活打死，更多的人则选择了用自杀的方式来维护自己的尊严。老舍、吴晗、葛伯赞、傅雷、赵九章、以群、闻捷、海默等，都自己结束了他们那曾经让人肃然起敬的生命。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从这一阶段幸存下来的人，在持续的残酷打击下渐渐麻木，这是一种自我保护的精神外壳，使他们避免最后的崩溃。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>他们在批斗会上常常进入半睡眠状态，只有一声恫吓才能使其惊醒过来，机械地重复那已说过无数遍的认罪词；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>然后，他们中的一部分人便进入了第三阶段，旷日持久的批判将鲜明的政治图像如水银般注入了他们的意识，将他们那由知识和理性构筑的思想大厦彻底摧毁，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>他们真的相信自己有罪，真的看到了自己对伟大事业构成的损害，并为此痛哭流涕，他们的忏悔往往比那些非知识分子的牛鬼蛇神要深刻得多，也真诚得多。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>而对于红卫兵来说，进入后两个阶段的批判对象是最乏味的，只有处于第一阶段的牛鬼蛇神才能对他们那早已过度兴奋的神经产生有效的刺激，如同斗牛士手上的红布，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>但这样的对象越来越少了，在这所大学中可能只剩下一个，他由于自己的珍稀而被留到批判大会最后出场。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -761,10 +981,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1073,6 +1293,160 @@
         <v>48</v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Site updated: 2025年9月24日 23:02:29
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE7BB8-378D-4A2C-AA14-2B0B025CC375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA70653-B938-4D9E-8A8F-831C18C73549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -984,7 +984,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Site updated: 2025年9月25日 23:59:57
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA70653-B938-4D9E-8A8F-831C18C73549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C252A0-60CC-4C73-AC1D-1AE4E75D07BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
   <si>
     <t>The Red Union had been attacking the headquarters of the April Twenty-eighth Brigade for two days. Their red flags fluttered restlessly around the brigade building like flames yearning for firewood.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -616,6 +616,168 @@
   <si>
     <t>但这样的对象越来越少了，在这所大学中可能只剩下一个，他由于自己的珍稀而被留到批判大会最后出场。</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>像这样的战斗席卷整个北京，就像大量的中央处理器并行工作，它们的联合输出，即文化大革命。疯狂的洪水淹没了这座城市，渗透到每个角落。</t>
+  </si>
+  <si>
+    <r>
+      <t>在城市的边缘，清华大学的操场上，一场有数千人参加的群众</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>斗争大会</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>已经持续了近两个小时。</t>
+    </r>
+  </si>
+  <si>
+    <t>这是一次公众集会，目的是通过言语和身体虐待来羞辱和瓦解革命的敌人，直到他们在群众面前承认他们的罪行。</t>
+  </si>
+  <si>
+    <t>由于革命者已经分裂成许多派别，各地的敌对势力都参与了复杂的演习和竞赛。在大学内部，红卫兵、文革工作组、工宣队、军宣队之间爆发了激烈的冲突。</t>
+  </si>
+  <si>
+    <t>每个派别不时分裂成新的反叛团体，每个团体都有不同的背景和议程，导致更加残酷的战斗。</t>
+  </si>
+  <si>
+    <t>但是对于这次群众斗争会议来说，受害者是反动的资产阶级学术当局。这些人是每个派别的敌人，他们别无选择，只能忍受来自四面八方的残酷攻击。</t>
+  </si>
+  <si>
+    <r>
+      <t>与其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>妖魔鬼怪</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>”</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>相比，反动学术权威是特殊的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>在最早的斗争时期，他们既傲慢又顽固。这也是他们死亡人数最多的阶段。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>在四十天的时间里，仅在北京，就有一千七百多名斗争会的受害者被打死。许多人选择了一条更容易的道路来避免这种疯狂</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>老舍、吴晗、翦伯赞、傅雷、赵九章、易群、文杰、海默和其他曾经受人尊敬的知识分子都选择了结束自己的生命</t>
+    </r>
+  </si>
+  <si>
+    <t>随着残酷斗争的继续，那些在初期幸存下来的人逐渐变得麻木。保护性的精神外壳帮助他们避免完全崩溃。</t>
+  </si>
+  <si>
+    <t>在治疗过程中，他们经常看起来半睡半醒，只有当有人在他们面前尖叫，让他们机械地背诵他们已经重复了无数次的供词时，他们才会惊醒。</t>
+  </si>
+  <si>
+    <t>然后，他们中的一些人进入了第三阶段。持续不断的斗争会议像水银一样将生动的政治图像注入他们的意识，直到他们建立在知识和理性基础上的头脑在攻击下崩溃。</t>
+  </si>
+  <si>
+    <t>他们开始真正相信他们是有罪的，看到他们如何损害了革命的伟大事业。他们哭了，他们的忏悔远比那些不是知识分子的妖魔鬼怪来得深刻和真诚。</t>
+  </si>
+  <si>
+    <t>对于红卫兵来说，在后两个心理阶段对受害者进行大量虐待是非常无聊的。只有那些仍处于初级阶段的怪物和恶魔才能给他们过度刺激的大脑带来他们渴望的刺激，就像斗牛士的红色斗篷。</t>
+  </si>
+  <si>
+    <t>但是这种理想的受害者越来越少了。清华大概只剩下一个了。因为他是如此罕见，他被保留到最后的斗争会议。</t>
   </si>
 </sst>
 </file>
@@ -664,15 +826,27 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -680,25 +854,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -983,15 +1184,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="3"/>
     <col min="3" max="3" width="31" style="3" customWidth="1"/>
-    <col min="4" max="6" width="40.77734375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="40.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="40.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="73.44140625" style="7" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -1106,10 +1309,10 @@
       <c r="D8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1126,10 +1329,10 @@
       <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1146,10 +1349,10 @@
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1166,10 +1369,10 @@
       <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1186,10 +1389,10 @@
       <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1206,10 +1409,10 @@
       <c r="D13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="8" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1226,10 +1429,10 @@
       <c r="D14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="8" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1246,10 +1449,10 @@
       <c r="D15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="8" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1266,10 +1469,10 @@
       <c r="D16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1278,7 +1481,7 @@
         <v>3.5763888888888889E-3</v>
       </c>
       <c r="B17" s="1">
-        <v>3.7152777777777778E-3</v>
+        <v>3.7037037037037038E-3</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>38</v>
@@ -1286,44 +1489,71 @@
       <c r="D17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="8" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>3.7268518518518519E-3</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3.9120370370370368E-3</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>82</v>
       </c>
+      <c r="F18" s="8" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3.9236111111111112E-3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.0509259259259257E-3</v>
+      </c>
       <c r="C19" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>83</v>
       </c>
+      <c r="F19" s="8" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>4.0625000000000001E-3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4.1898148148148146E-3</v>
+      </c>
       <c r="C20" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="4" t="s">
         <v>84</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,8 +1563,11 @@
       <c r="D21" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>85</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1344,8 +1577,11 @@
       <c r="D22" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="5" t="s">
         <v>86</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1355,8 +1591,11 @@
       <c r="D23" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>87</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1366,8 +1605,11 @@
       <c r="D24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="5" t="s">
         <v>88</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1377,8 +1619,11 @@
       <c r="D25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>89</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1388,8 +1633,11 @@
       <c r="D26" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="5" t="s">
         <v>90</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,8 +1647,11 @@
       <c r="D27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="5" t="s">
         <v>91</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,8 +1661,11 @@
       <c r="D28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="5" t="s">
         <v>92</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,8 +1675,11 @@
       <c r="D29" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>93</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1432,8 +1689,11 @@
       <c r="D30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="5" t="s">
         <v>94</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1443,8 +1703,11 @@
       <c r="D31" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="5" t="s">
         <v>95</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2025年9月28日 22:48:11
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C252A0-60CC-4C73-AC1D-1AE4E75D07BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722ADF03-C6D4-4871-ADE6-CA54DF350EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -667,9 +667,6 @@
     <t>这是一次公众集会，目的是通过言语和身体虐待来羞辱和瓦解革命的敌人，直到他们在群众面前承认他们的罪行。</t>
   </si>
   <si>
-    <t>由于革命者已经分裂成许多派别，各地的敌对势力都参与了复杂的演习和竞赛。在大学内部，红卫兵、文革工作组、工宣队、军宣队之间爆发了激烈的冲突。</t>
-  </si>
-  <si>
     <t>每个派别不时分裂成新的反叛团体，每个团体都有不同的背景和议程，导致更加残酷的战斗。</t>
   </si>
   <si>
@@ -778,6 +775,10 @@
   </si>
   <si>
     <t>但是这种理想的受害者越来越少了。清华大概只剩下一个了。因为他是如此罕见，他被保留到最后的斗争会议。</t>
+  </si>
+  <si>
+    <t>由于革命者分裂成众多派系，各地反对势力展开了复杂的博弈与角逐。在大学内部，红卫兵、文化大革命工作组、工人宣传队和军事宣传队之间爆发了激烈冲突。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1184,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1557,6 +1558,12 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>4.2013888888888891E-3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4.43287037037037E-3</v>
+      </c>
       <c r="C21" s="2" t="s">
         <v>71</v>
       </c>
@@ -1567,10 +1574,16 @@
         <v>85</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>4.43287037037037E-3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4.5601851851851853E-3</v>
+      </c>
       <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
@@ -1581,10 +1594,16 @@
         <v>86</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>4.5717592592592589E-3</v>
+      </c>
+      <c r="B23" s="1">
+        <v>4.7569444444444447E-3</v>
+      </c>
       <c r="C23" s="2" t="s">
         <v>73</v>
       </c>
@@ -1595,10 +1614,16 @@
         <v>87</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>4.7685185185185183E-3</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4.9884259259259257E-3</v>
+      </c>
       <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
@@ -1609,10 +1634,16 @@
         <v>88</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>4.9884259259259257E-3</v>
+      </c>
+      <c r="B25" s="1">
+        <v>5.324074074074074E-3</v>
+      </c>
       <c r="C25" s="2" t="s">
         <v>75</v>
       </c>
@@ -1623,10 +1654,16 @@
         <v>89</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>5.347222222222222E-3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5.4861111111111109E-3</v>
+      </c>
       <c r="C26" s="2" t="s">
         <v>76</v>
       </c>
@@ -1637,10 +1674,16 @@
         <v>90</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>5.4861111111111109E-3</v>
+      </c>
+      <c r="B27" s="1">
+        <v>5.6365740740740742E-3</v>
+      </c>
       <c r="C27" s="2" t="s">
         <v>77</v>
       </c>
@@ -1651,10 +1694,16 @@
         <v>91</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>5.6365740740740742E-3</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5.8680555555555552E-3</v>
+      </c>
       <c r="C28" s="2" t="s">
         <v>78</v>
       </c>
@@ -1665,10 +1714,16 @@
         <v>92</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>5.8680555555555552E-3</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.076388888888889E-3</v>
+      </c>
       <c r="C29" s="2" t="s">
         <v>79</v>
       </c>
@@ -1679,10 +1734,16 @@
         <v>93</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>6.0879629629629626E-3</v>
+      </c>
+      <c r="B30" s="1">
+        <v>6.2847222222222219E-3</v>
+      </c>
       <c r="C30" s="2" t="s">
         <v>80</v>
       </c>
@@ -1693,10 +1754,16 @@
         <v>94</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>6.2962962962962964E-3</v>
+      </c>
+      <c r="B31" s="1">
+        <v>6.4467592592592588E-3</v>
+      </c>
       <c r="C31" s="2" t="s">
         <v>81</v>
       </c>
@@ -1707,7 +1774,7 @@
         <v>95</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2025年10月2日 09:19:33
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{722ADF03-C6D4-4871-ADE6-CA54DF350EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7AFA35-4EA8-4A36-AB75-86B472C0AB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
   <si>
     <t>The Red Union had been attacking the headquarters of the April Twenty-eighth Brigade for two days. Their red flags fluttered restlessly around the brigade building like flames yearning for firewood.</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -778,6 +778,18 @@
   </si>
   <si>
     <t>由于革命者分裂成众多派系，各地反对势力展开了复杂的博弈与角逐。在大学内部，红卫兵、文化大革命工作组、工人宣传队和军事宣传队之间爆发了激烈冲突。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:06:23.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:09:17.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:09:04.5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -874,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -901,6 +913,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1185,8 +1200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1561,8 +1576,8 @@
       <c r="A21" s="1">
         <v>4.2013888888888891E-3</v>
       </c>
-      <c r="B21" s="1">
-        <v>4.43287037037037E-3</v>
+      <c r="B21" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>71</v>
@@ -1578,8 +1593,8 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>4.43287037037037E-3</v>
+      <c r="A22" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="B22" s="1">
         <v>4.5601851851851853E-3</v>
@@ -1742,7 +1757,7 @@
         <v>6.0879629629629626E-3</v>
       </c>
       <c r="B30" s="1">
-        <v>6.2847222222222219E-3</v>
+        <v>6.2962962962962964E-3</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>80</v>
@@ -1758,11 +1773,11 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>6.2962962962962964E-3</v>
-      </c>
-      <c r="B31" s="1">
-        <v>6.4467592592592588E-3</v>
+      <c r="A31" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>111</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Site updated: 2025年10月3日 19:03:54
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7AFA35-4EA8-4A36-AB75-86B472C0AB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47333C8B-1EC7-4280-A929-719E2F7E099C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,8 +735,42 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>在四十天的时间里，仅在北京，就有一千七百多名斗争会的受害者被打死。许多人选择了一条更容易的道路来避免这种疯狂</t>
+    <t>随着残酷斗争的继续，那些在初期幸存下来的人逐渐变得麻木。保护性的精神外壳帮助他们避免完全崩溃。</t>
+  </si>
+  <si>
+    <t>在治疗过程中，他们经常看起来半睡半醒，只有当有人在他们面前尖叫，让他们机械地背诵他们已经重复了无数次的供词时，他们才会惊醒。</t>
+  </si>
+  <si>
+    <t>然后，他们中的一些人进入了第三阶段。持续不断的斗争会议像水银一样将生动的政治图像注入他们的意识，直到他们建立在知识和理性基础上的头脑在攻击下崩溃。</t>
+  </si>
+  <si>
+    <t>他们开始真正相信他们是有罪的，看到他们如何损害了革命的伟大事业。他们哭了，他们的忏悔远比那些不是知识分子的妖魔鬼怪来得深刻和真诚。</t>
+  </si>
+  <si>
+    <t>对于红卫兵来说，在后两个心理阶段对受害者进行大量虐待是非常无聊的。只有那些仍处于初级阶段的怪物和恶魔才能给他们过度刺激的大脑带来他们渴望的刺激，就像斗牛士的红色斗篷。</t>
+  </si>
+  <si>
+    <t>但是这种理想的受害者越来越少了。清华大概只剩下一个了。因为他是如此罕见，他被保留到最后的斗争会议。</t>
+  </si>
+  <si>
+    <t>由于革命者分裂成众多派系，各地反对势力展开了复杂的博弈与角逐。在大学内部，红卫兵、文化大革命工作组、工人宣传队和军事宣传队之间爆发了激烈冲突。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:06:23.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:09:17.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0:09:04.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>在四十多天的时间里，仅在北京就有一千七百多名斗争会的受害者被殴打致死。还有许多人选择了一条更轻松的道路来躲避疯狂：</t>
     </r>
     <r>
       <rPr>
@@ -745,51 +779,19 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>老舍、吴晗、翦伯赞、傅雷、赵九章、易群、文杰、海默和其他曾经受人尊敬的知识分子都选择了结束自己的生命</t>
-    </r>
-  </si>
-  <si>
-    <t>随着残酷斗争的继续，那些在初期幸存下来的人逐渐变得麻木。保护性的精神外壳帮助他们避免完全崩溃。</t>
-  </si>
-  <si>
-    <t>在治疗过程中，他们经常看起来半睡半醒，只有当有人在他们面前尖叫，让他们机械地背诵他们已经重复了无数次的供词时，他们才会惊醒。</t>
-  </si>
-  <si>
-    <t>然后，他们中的一些人进入了第三阶段。持续不断的斗争会议像水银一样将生动的政治图像注入他们的意识，直到他们建立在知识和理性基础上的头脑在攻击下崩溃。</t>
-  </si>
-  <si>
-    <t>他们开始真正相信他们是有罪的，看到他们如何损害了革命的伟大事业。他们哭了，他们的忏悔远比那些不是知识分子的妖魔鬼怪来得深刻和真诚。</t>
-  </si>
-  <si>
-    <t>对于红卫兵来说，在后两个心理阶段对受害者进行大量虐待是非常无聊的。只有那些仍处于初级阶段的怪物和恶魔才能给他们过度刺激的大脑带来他们渴望的刺激，就像斗牛士的红色斗篷。</t>
-  </si>
-  <si>
-    <t>但是这种理想的受害者越来越少了。清华大概只剩下一个了。因为他是如此罕见，他被保留到最后的斗争会议。</t>
-  </si>
-  <si>
-    <t>由于革命者分裂成众多派系，各地反对势力展开了复杂的博弈与角逐。在大学内部，红卫兵、文化大革命工作组、工人宣传队和军事宣传队之间爆发了激烈冲突。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:06:23.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:09:17.5</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0:09:04.5</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">老舍、吴晗、翦伯赞、傅雷、赵九章、易群、闻捷、海默等曾经受人尊敬的知识分子都选择了结束自己的生命。
+</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -886,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -917,6 +919,9 @@
     </xf>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1200,8 +1205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1577,7 +1582,7 @@
         <v>4.2013888888888891E-3</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>71</v>
@@ -1589,12 +1594,12 @@
         <v>85</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B22" s="1">
         <v>4.5601851851851853E-3</v>
@@ -1668,8 +1673,8 @@
       <c r="E25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>102</v>
+      <c r="F25" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1689,7 +1694,7 @@
         <v>90</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,7 +1714,7 @@
         <v>91</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1729,7 +1734,7 @@
         <v>92</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1749,7 +1754,7 @@
         <v>93</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1769,15 +1774,15 @@
         <v>94</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>81</v>
@@ -1789,7 +1794,7 @@
         <v>95</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2025年10月4日 22:53:42
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47333C8B-1EC7-4280-A929-719E2F7E099C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1B5206-17F8-4A84-90F6-D05301ADC61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,9 +735,6 @@
     </r>
   </si>
   <si>
-    <t>随着残酷斗争的继续，那些在初期幸存下来的人逐渐变得麻木。保护性的精神外壳帮助他们避免完全崩溃。</t>
-  </si>
-  <si>
     <t>在治疗过程中，他们经常看起来半睡半醒，只有当有人在他们面前尖叫，让他们机械地背诵他们已经重复了无数次的供词时，他们才会惊醒。</t>
   </si>
   <si>
@@ -793,6 +790,9 @@
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随着残酷斗争的继续，那些在最初阶段幸存下来的人逐渐变得麻木，精神保护壳帮助他们避免了彻底崩溃。</t>
   </si>
 </sst>
 </file>
@@ -888,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -919,9 +919,6 @@
     </xf>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1206,7 +1203,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1582,7 +1579,7 @@
         <v>4.2013888888888891E-3</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>71</v>
@@ -1594,12 +1591,12 @@
         <v>85</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="1">
         <v>4.5601851851851853E-3</v>
@@ -1673,8 +1670,8 @@
       <c r="E25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>112</v>
+      <c r="F25" s="8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1694,7 +1691,7 @@
         <v>90</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1714,7 +1711,7 @@
         <v>91</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1734,7 +1731,7 @@
         <v>92</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1754,7 +1751,7 @@
         <v>93</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1774,15 +1771,15 @@
         <v>94</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>81</v>
@@ -1794,7 +1791,7 @@
         <v>95</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2025年10月8日 23:49:37
</commit_message>
<xml_diff>
--- a/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
+++ b/THE_THREE_BODY_PROBLEM_Audio_Book/1-1疯狂年代_The_Madness_Years.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Blogs\my-blog\source\THE_THREE_BODY_PROBLEM_Audio_Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1B5206-17F8-4A84-90F6-D05301ADC61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E672257F-48A7-480D-A63B-9851514AC2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,19 +735,7 @@
     </r>
   </si>
   <si>
-    <t>在治疗过程中，他们经常看起来半睡半醒，只有当有人在他们面前尖叫，让他们机械地背诵他们已经重复了无数次的供词时，他们才会惊醒。</t>
-  </si>
-  <si>
-    <t>然后，他们中的一些人进入了第三阶段。持续不断的斗争会议像水银一样将生动的政治图像注入他们的意识，直到他们建立在知识和理性基础上的头脑在攻击下崩溃。</t>
-  </si>
-  <si>
     <t>他们开始真正相信他们是有罪的，看到他们如何损害了革命的伟大事业。他们哭了，他们的忏悔远比那些不是知识分子的妖魔鬼怪来得深刻和真诚。</t>
-  </si>
-  <si>
-    <t>对于红卫兵来说，在后两个心理阶段对受害者进行大量虐待是非常无聊的。只有那些仍处于初级阶段的怪物和恶魔才能给他们过度刺激的大脑带来他们渴望的刺激，就像斗牛士的红色斗篷。</t>
-  </si>
-  <si>
-    <t>但是这种理想的受害者越来越少了。清华大概只剩下一个了。因为他是如此罕见，他被保留到最后的斗争会议。</t>
   </si>
   <si>
     <t>由于革命者分裂成众多派系，各地反对势力展开了复杂的博弈与角逐。在大学内部，红卫兵、文化大革命工作组、工人宣传队和军事宣传队之间爆发了激烈冲突。</t>
@@ -793,6 +781,26 @@
   </si>
   <si>
     <t>随着残酷斗争的继续，那些在最初阶段幸存下来的人逐渐变得麻木，精神保护壳帮助他们避免了彻底崩溃。</t>
+  </si>
+  <si>
+    <t>然后，他们中的一些人进入了第三阶段。持续不断的斗争会议像水银一样将生动的政治图像注入他们的意识，直到他们建立在知识和理性基础上的头脑在攻击下崩溃。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在治疗过程中，他们经常看起来半睡半醒，只有当有人在他们面前尖叫，让他们机械地背诵他们已经重复了无数次的供词时，他们才会惊醒。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">对于红卫兵来说，在后两个心理阶段对受害者进行大量虐待是非常无聊的。只有那些仍处于初级阶段的怪物和恶魔才能给他们过度刺激的大脑带来他们渴望的刺激，就像斗牛士的红色斗篷。
+对于红卫兵来说，对处于后两个精神阶段的受害者进行虐待是非常无聊的。只有那些仍处于初始阶段的妖魔鬼怪才能给他们过度兴奋的大脑带来他们渴望的刺激，就像斗牛士的红色斗篷一样。
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">但是这种理想的受害者越来越少了。清华大概只剩下一个了。因为他是如此罕见，他被保留到最后的斗争会议。
+但这种理想的牺牲品已经越来越少了。在清华，可能只剩下一个了。因为他太稀有了，所以被保留到了斗争会的最后。
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -888,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -919,6 +927,9 @@
     </xf>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1202,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1579,7 +1590,7 @@
         <v>4.2013888888888891E-3</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>71</v>
@@ -1591,12 +1602,12 @@
         <v>85</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B22" s="1">
         <v>4.5601851851851853E-3</v>
@@ -1671,7 +1682,7 @@
         <v>89</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1691,7 +1702,7 @@
         <v>90</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1711,7 +1722,7 @@
         <v>91</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1731,7 +1742,7 @@
         <v>92</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1751,7 +1762,7 @@
         <v>93</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,16 +1781,16 @@
       <c r="E30" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="8" t="s">
-        <v>105</v>
+      <c r="F30" s="11" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>81</v>
@@ -1790,8 +1801,8 @@
       <c r="E31" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>106</v>
+      <c r="F31" s="11" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>